<commit_message>
Customer Contact Job Update
</commit_message>
<xml_diff>
--- a/Folder/Automation Test Data.xlsx
+++ b/Folder/Automation Test Data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zaigo PC\eclipse-workspace\Fieldy_Zaiportal_New\Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD616AE2-AA26-4B52-A830-CF9BEB0F8707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C4482E-1E6B-4C7D-BA9B-BF5BFC984392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{FF98523A-AACE-4AD2-896B-F8F356C94E92}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{FF98523A-AACE-4AD2-896B-F8F356C94E92}"/>
   </bookViews>
   <sheets>
     <sheet name="Tenant Customer" sheetId="1" r:id="rId1"/>
     <sheet name="Team User" sheetId="2" r:id="rId2"/>
     <sheet name="Team Details Screen" sheetId="4" r:id="rId3"/>
-    <sheet name="NumberGenerate" sheetId="3" r:id="rId4"/>
+    <sheet name="Onboarding" sheetId="5" r:id="rId4"/>
+    <sheet name="NumberGenerate" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3332,7 +3333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982BDF5D-7751-43DE-8A7A-BF65676424C5}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -3525,6 +3526,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57427788-7EB6-4DEF-B519-03F4FBE9C48A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A9B07E-3A91-4050-94FA-6A005CB0898A}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>